<commit_message>
Product adding using excel
</commit_message>
<xml_diff>
--- a/Empirehomecrm/src/main/java/com/testdata/EhUsernames.xlsx
+++ b/Empirehomecrm/src/main/java/com/testdata/EhUsernames.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18600" windowHeight="6950"/>
+    <workbookView windowWidth="19200" windowHeight="6950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="multipleusernames" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>username</t>
   </si>
@@ -29,6 +30,45 @@
   </si>
   <si>
     <t>sureshbabuemp</t>
+  </si>
+  <si>
+    <t>ModelNumber</t>
+  </si>
+  <si>
+    <t>ItemTitle</t>
+  </si>
+  <si>
+    <t>ItemDescription</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Breadth</t>
+  </si>
+  <si>
+    <t>ColorName</t>
+  </si>
+  <si>
+    <t>ActualPrice</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>XYZ420</t>
+  </si>
+  <si>
+    <t>Dinning Table</t>
+  </si>
+  <si>
+    <t>With Four Chairs</t>
+  </si>
+  <si>
+    <t>Black</t>
   </si>
 </sst>
 </file>
@@ -644,12 +684,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1189,7 +1226,7 @@
   <sheetPr/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
@@ -1242,10 +1279,97 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>12345</v>
       </c>
       <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="14.7272727272727" customWidth="1"/>
+    <col min="2" max="2" width="30.0909090909091" customWidth="1"/>
+    <col min="3" max="3" width="16.4545454545455" customWidth="1"/>
+    <col min="4" max="4" width="16.8181818181818" customWidth="1"/>
+    <col min="5" max="5" width="16.4545454545455" customWidth="1"/>
+    <col min="6" max="6" width="18.1818181818182" customWidth="1"/>
+    <col min="7" max="7" width="12.0909090909091" customWidth="1"/>
+    <col min="8" max="8" width="11.3636363636364" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="21.2727272727273" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2">
+        <v>30000</v>
+      </c>
+      <c r="I2">
         <v>3</v>
       </c>
     </row>

</xml_diff>